<commit_message>
Added TC003, Fixed TC001 and TC002, Removed TestScrolling.java
</commit_message>
<xml_diff>
--- a/Test Cases/Test Case.xlsx
+++ b/Test Cases/Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chirag.Bitoni\IdeaProjects\SeleniumJavaAutomationFramework\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44006146-F34F-4D95-B8FE-F042EEEE7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3457F3D-1CA2-4FD4-82A2-0025A821ED1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -85,13 +85,24 @@
     <t>Navigate to the Check Box page</t>
   </si>
   <si>
+    <t>Selected/deselected items should display in the output list.</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Checkbox State</t>
+  </si>
+  <si>
+    <t>Verify checkbox state changes correctly after pressing checking/unchecking.</t>
+  </si>
+  <si>
     <t>1. Expand the Home Folder.
 2. Click the checkbox of "Home" checkbox.
-3. Click the checkbox of "Documents" checkbox.
-4. Verify checked state of checkbox.</t>
-  </si>
-  <si>
-    <t>Selected/deselected items should display in the output list.</t>
+3. Click the checkbox of "Documents" checkbox.</t>
+  </si>
+  <si>
+    <t>Checked state of checkbox should be displayed correctly.</t>
   </si>
 </sst>
 </file>
@@ -436,11 +447,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +515,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -518,12 +529,35 @@
         <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added TC006 & TC007
</commit_message>
<xml_diff>
--- a/Test Cases/Test Case.xlsx
+++ b/Test Cases/Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chirag.Bitoni\IdeaProjects\SeleniumJavaAutomationFramework\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E0C70-C208-4F93-A9FC-E6F88C62E67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0951A654-8EAB-401C-AAB8-A537D3719A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -149,6 +149,45 @@
 Modify a field (e.g., Salary) and click "Submit".
 6. Locate the same record.
 7. Click the "Delete" button.</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Search and Reset Functionality</t>
+  </si>
+  <si>
+    <t>Verify that the search and reset functionalities work correctly.</t>
+  </si>
+  <si>
+    <t>1. Enter a search term (e.g., First Name or Department).
+2.Verify that only matching records are displayed.
+3. Clear the search input field and verify that the table displays all records.
+4. Test case-insensitivity by searching with uppercase and lowercase terms (e.g., "JOHN" vs. "john").</t>
+  </si>
+  <si>
+    <t>The table filters records accurately based on the search term.
+Clearing the search resets the table to show all records.
+Search functionality is case insensitive.</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>Verify that sorting works correctly.</t>
+  </si>
+  <si>
+    <t>1. Click any column header to apply sorting.
+2. Verify that tab;e is sortedin ascending and descending order for each column.</t>
+  </si>
+  <si>
+    <t>Sorting work as expected and coirrect records are displayed.</t>
+  </si>
+  <si>
+    <t>TC008</t>
   </si>
 </sst>
 </file>
@@ -496,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +691,60 @@
       <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">

</xml_diff>

<commit_message>
Added TC010 and TC011
</commit_message>
<xml_diff>
--- a/Test Cases/Test Case.xlsx
+++ b/Test Cases/Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chirag.Bitoni\IdeaProjects\SeleniumJavaAutomationFramework\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580604F6-F644-4AE5-AEB8-FBA712D4443E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23F8BC0-33F4-4BB5-835B-CF3F015195A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -230,6 +230,42 @@
   <si>
     <t>Navigation links open in a new tab with the correct URL.
 API links display the expected status codes and messages.</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>Valid and Broken Images</t>
+  </si>
+  <si>
+    <t>Valid and Broken Links</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>Verify that both broken and non-broken images are correctly identified on the page.</t>
+  </si>
+  <si>
+    <t>Navigate to Broken Links-Images page.</t>
+  </si>
+  <si>
+    <t>Verify that the valid link redirects to the correct page and the broken link results in an error page.</t>
+  </si>
+  <si>
+    <t>1. Check whether the  'naturalWidth' Attribute is equal to 0 or not.</t>
+  </si>
+  <si>
+    <t>1. Open the links with Ctrl+Click.
+2. Verify the response code.</t>
+  </si>
+  <si>
+    <t>The valid image should have a naturalWidth greater than 0, meaning it is displayed correctly.
+The broken image should have a naturalWidth of 0, indicating it is not displayed.</t>
+  </si>
+  <si>
+    <t>The valid link should open in a new tab and load successfully with an HTTP 200 status code.
+The broken link should open in a new tab and return an HTTP 500 status code (indicating an error page).</t>
   </si>
 </sst>
 </file>
@@ -577,19 +613,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -826,6 +862,52 @@
         <v>58</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>